<commit_message>
Added advatages on all pages with doors
</commit_message>
<xml_diff>
--- a/Преимущества дверей.xlsx
+++ b/Преимущества дверей.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14100" windowHeight="9072"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Деревянные двери</t>
   </si>
@@ -82,6 +82,9 @@
     <t>Теплопроводность</t>
   </si>
   <si>
+    <t>Двери из лситвенницы обладают повышенным тепловым сопротивленим, что крайне полезно в холодный, сезонный период, когда используется отопление</t>
+  </si>
+  <si>
     <t xml:space="preserve">Нагрузка на створки </t>
   </si>
   <si>
@@ -140,6 +143,64 @@
   </si>
   <si>
     <t>В этом разделе, в преимуществах, можно часто видеть "благодаря прияродной стрктуре". Мы стараемся выделить преимущества каждого материала, чтобы клиент, исходят из своих пожеланий мог выбрать вариант, удовлетворяющий основным требованиям. VitHouse никак не может повлиять на природные преимущества материалов, однако, может гарантировать клиентам, что их продукция будет произведена из материалов самого высокого качества, обладающими всеми перечисленными преимуществами</t>
+  </si>
+  <si>
+    <t>Уникальность профиля</t>
+  </si>
+  <si>
+    <t>Преимущества по материалу</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>Деревянный профиль с классической фрезеровкой без стекляных и металических элементов. Для тех, кто ценит классический стиль, его постоянство и фундаментальность</t>
+  </si>
+  <si>
+    <t>Сосна</t>
+  </si>
+  <si>
+    <t>AL Classic</t>
+  </si>
+  <si>
+    <t>Дерево-алюминиевая конструкция классической двери. Наружный алюминиевый профиль рамы, створки и филенки имеет специальную форму</t>
+  </si>
+  <si>
+    <t>DV Contour AL</t>
+  </si>
+  <si>
+    <t>Алюминиевый профиль имеют строго прямоугольную форму. Рамный и створочный профиль со стороны улицы находятся в одной плоскости</t>
+  </si>
+  <si>
+    <t>DV MODERN</t>
+  </si>
+  <si>
+    <t>Уникальность профиля заключается в необычной, свойственной только этому типу фрезировке. Не имеет отличий по техническим характеристикам относительно других наших дверей</t>
+  </si>
+  <si>
+    <t>DV MODERN AL</t>
+  </si>
+  <si>
+    <t>Дерево-алюминиевая конструкция щитовой двери. Отличается накладкой из алюминиевого листа со стороны улицы и собственным уникальным стилем</t>
+  </si>
+  <si>
+    <t>DV Optima</t>
+  </si>
+  <si>
+    <t>Отличительной особенностью профиля является внешний вид . По техническим характеристикам не уступает и не превосходит наши двери с другими типами профилей</t>
+  </si>
+  <si>
+    <t>DV Optima AL</t>
+  </si>
+  <si>
+    <t>Входная дверь дерево-алюминиевой конструкции на базе профиля Optima - алюминивые накладки повторяют форму основы из дерева</t>
+  </si>
+  <si>
+    <t>DV Rustic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Входные деревянные двери в профиле RUSTIC заинтересуют людей, которые решили оформить фасад загородного дома в деревенском стиле, стиле кантри или прованс
+</t>
   </si>
 </sst>
 </file>
@@ -147,10 +208,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -170,6 +231,67 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,60 +322,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,29 +360,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,31 +375,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,25 +495,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,121 +519,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,17 +791,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -750,15 +805,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -781,8 +827,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,17 +870,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -832,152 +893,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1061,6 +1122,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1381,10 +1448,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1610,7 +1677,7 @@
         <v>21</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K7" s="19"/>
       <c r="L7" s="27"/>
@@ -1709,28 +1776,28 @@
         <v>13</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K11" s="19"/>
       <c r="L11" s="27"/>
@@ -1823,34 +1890,34 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="27"/>
@@ -1943,23 +2010,23 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="27"/>
@@ -2076,11 +2143,15 @@
       <c r="V23" s="27"/>
       <c r="W23" s="27"/>
     </row>
-    <row r="24" spans="1:23">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
+    <row r="24" ht="70" customHeight="1" spans="1:23">
+      <c r="A24" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="9"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
@@ -2102,10 +2173,18 @@
       <c r="W24" s="27"/>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
+      <c r="A25" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
@@ -2127,10 +2206,10 @@
       <c r="W25" s="27"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
@@ -2152,10 +2231,10 @@
       <c r="W26" s="27"/>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
@@ -2177,10 +2256,10 @@
       <c r="W27" s="27"/>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
@@ -2202,9 +2281,13 @@
       <c r="W28" s="27"/>
     </row>
     <row r="29" spans="1:23">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="9"/>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
@@ -2227,9 +2310,9 @@
       <c r="W29" s="27"/>
     </row>
     <row r="30" spans="1:23">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
@@ -2252,9 +2335,9 @@
       <c r="W30" s="27"/>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
@@ -2277,9 +2360,9 @@
       <c r="W31" s="27"/>
     </row>
     <row r="32" spans="1:23">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
@@ -2302,8 +2385,12 @@
       <c r="W32" s="27"/>
     </row>
     <row r="33" spans="1:23">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
@@ -2327,8 +2414,8 @@
       <c r="W33" s="27"/>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="27"/>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
@@ -2352,8 +2439,8 @@
       <c r="W34" s="27"/>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
@@ -2377,8 +2464,8 @@
       <c r="W35" s="27"/>
     </row>
     <row r="36" spans="1:23">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
@@ -2402,8 +2489,12 @@
       <c r="W36" s="27"/>
     </row>
     <row r="37" spans="1:23">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="C37" s="27"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
@@ -2427,8 +2518,8 @@
       <c r="W37" s="27"/>
     </row>
     <row r="38" spans="1:23">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="27"/>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
@@ -2451,29 +2542,138 @@
       <c r="V38" s="27"/>
       <c r="W38" s="27"/>
     </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="19"/>
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" ht="29" customHeight="1" spans="1:2">
+      <c r="A40" s="19"/>
+      <c r="B40" s="9"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="28"/>
+      <c r="B42" s="29"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="28"/>
+      <c r="B43" s="29"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="28"/>
+      <c r="B44" s="29"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="28"/>
+      <c r="B46" s="29"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="28"/>
+      <c r="B47" s="29"/>
+    </row>
+    <row r="48" ht="31" customHeight="1" spans="1:2">
+      <c r="A48" s="28"/>
+      <c r="B48" s="29"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="29"/>
+      <c r="B54" s="28"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="29"/>
+      <c r="B55" s="28"/>
+    </row>
+    <row r="56" ht="28" customHeight="1" spans="1:2">
+      <c r="A56" s="29"/>
+      <c r="B56" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="71">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A56"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B53:B56"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="C29:C32"/>
     <mergeCell ref="D2:D6"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="D15:D18"/>
+    <mergeCell ref="D25:D28"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="E7:E10"/>
     <mergeCell ref="E11:E14"/>

</xml_diff>